<commit_message>
added voltage regulator to VCF
</commit_message>
<xml_diff>
--- a/KiCAD/VCF/VCF BOM.xlsx
+++ b/KiCAD/VCF/VCF BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Kayne\Documents\KiCAD\Modular Synth\VCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{83287FB0-CF80-45E8-B142-E03EB3FD0FDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA34A818-36DE-471B-AEEB-EF2590477BC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VCF" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="107">
   <si>
     <t>Item</t>
   </si>
@@ -124,9 +132,6 @@
     <t>TL072</t>
   </si>
   <si>
-    <t>C1, C8, C11</t>
-  </si>
-  <si>
     <t>R1, R2</t>
   </si>
   <si>
@@ -142,9 +147,6 @@
     <t>RV1, RV3</t>
   </si>
   <si>
-    <t>C3-C7, C9, C10</t>
-  </si>
-  <si>
     <t>J2-J4</t>
   </si>
   <si>
@@ -314,12 +316,45 @@
   </si>
   <si>
     <t>https://www.digikey.com/short/pzvv0r</t>
+  </si>
+  <si>
+    <t>C3-C7, C9, C10, C14, C15</t>
+  </si>
+  <si>
+    <t>C1, C8, C11-C13</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>L78L09</t>
+  </si>
+  <si>
+    <t>L79L09</t>
+  </si>
+  <si>
+    <t>SOT-89</t>
+  </si>
+  <si>
+    <t>497-1192-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/short/pz1hnp</t>
+  </si>
+  <si>
+    <t>NJM79L09UA-TE1CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/short/pz1hn5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1162,19 +1197,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.90625" customWidth="1"/>
     <col min="2" max="2" width="4.81640625" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" customWidth="1"/>
     <col min="5" max="5" width="11.6328125" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" style="1"/>
     <col min="7" max="7" width="12.1796875" style="1" customWidth="1"/>
@@ -1198,23 +1233,23 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="K1" s="3">
         <f>SUM(G2:G39)</f>
-        <v>20.510000000000009</v>
+        <v>22.346000000000011</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1222,29 +1257,29 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1">
         <v>0.22</v>
       </c>
       <c r="G2" s="1">
         <f>SUM(F2*B2)</f>
-        <v>0.66</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1261,7 +1296,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" s="1">
         <v>2.71</v>
@@ -1271,10 +1306,10 @@
         <v>2.71</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1282,29 +1317,29 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.61599999999999999</v>
+        <v>0.79199999999999993</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1321,7 +1356,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1">
         <v>0.28000000000000003</v>
@@ -1331,10 +1366,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1345,13 +1380,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1">
         <v>1.5</v>
@@ -1361,10 +1396,10 @@
         <v>4.5</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1381,7 +1416,7 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7" s="1">
         <v>0.24</v>
@@ -1391,10 +1426,10 @@
         <v>0.24</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1405,13 +1440,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1">
         <v>0.66800000000000004</v>
@@ -1421,10 +1456,10 @@
         <v>6.6800000000000006</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1441,7 +1476,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" s="1">
         <v>0.21</v>
@@ -1451,10 +1486,10 @@
         <v>0.21</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1465,13 +1500,13 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1">
         <v>0.1</v>
@@ -1481,10 +1516,10 @@
         <v>0.2</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1495,13 +1530,13 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1">
         <v>7.0000000000000007E-2</v>
@@ -1511,10 +1546,10 @@
         <v>0.21000000000000002</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1531,7 +1566,7 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F12" s="1">
         <v>0.1</v>
@@ -1541,10 +1576,10 @@
         <v>0.1</v>
       </c>
       <c r="H12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1561,7 +1596,7 @@
         <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1">
         <v>0.1</v>
@@ -1571,10 +1606,10 @@
         <v>0.1</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1585,13 +1620,13 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F14" s="1">
         <v>9.2999999999999999E-2</v>
@@ -1601,10 +1636,10 @@
         <v>0.74399999999999999</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1615,13 +1650,13 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15" s="1">
         <v>0.1</v>
@@ -1631,10 +1666,10 @@
         <v>0.2</v>
       </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1645,13 +1680,13 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F16" s="1">
         <v>0.1</v>
@@ -1661,10 +1696,10 @@
         <v>0.2</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1678,10 +1713,10 @@
         <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F17" s="1">
         <v>0.1</v>
@@ -1691,10 +1726,10 @@
         <v>0.1</v>
       </c>
       <c r="H17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1711,7 +1746,7 @@
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F18" s="1">
         <v>0.1</v>
@@ -1721,10 +1756,10 @@
         <v>0.1</v>
       </c>
       <c r="H18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1735,13 +1770,13 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
         <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F19" s="1">
         <v>0.79</v>
@@ -1751,10 +1786,10 @@
         <v>1.58</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1771,7 +1806,7 @@
         <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F20" s="1">
         <v>0.46</v>
@@ -1781,10 +1816,10 @@
         <v>0.46</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1801,7 +1836,7 @@
         <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21" s="1">
         <v>0.62</v>
@@ -1811,22 +1846,70 @@
         <v>0.62</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.42</v>
+      </c>
       <c r="G22" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.42</v>
+      </c>
+      <c r="H22" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.8</v>
+      </c>
       <c r="G23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>